<commit_message>
OpenWeather_GSheets_ReportBot: InitAllApplications workflow and Config Settings Worksheet updated
</commit_message>
<xml_diff>
--- a/uipath-projects/OpenWeather_GSheets_ReportBot/Data/Config.xlsx
+++ b/uipath-projects/OpenWeather_GSheets_ReportBot/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Giancarlo\GitHub\automation-ai-portfolio\uipath-projects\OpenWeather_GSheets_ReportBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8FA837-9AA4-4188-8768-5D9FE803F132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,36 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>WeatherAPIKey</t>
+  </si>
+  <si>
+    <t>WeatherAPIKey_AssetName</t>
+  </si>
+  <si>
+    <t>GoogleCredential</t>
+  </si>
+  <si>
+    <t>GoogleCredential_AssetName</t>
+  </si>
+  <si>
+    <t>InputCitiesPath</t>
+  </si>
+  <si>
+    <t>Data\InputCities.xlsx</t>
+  </si>
+  <si>
+    <t>InputCitiesFileSheet</t>
+  </si>
+  <si>
+    <t>Cities</t>
+  </si>
+  <si>
+    <t>OrchestratorFolderPath</t>
+  </si>
+  <si>
+    <t>GSFolder</t>
   </si>
 </sst>
 </file>
@@ -212,10 +242,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -239,9 +269,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +309,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +415,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,11 +567,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
@@ -615,9 +645,30 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1623,7 +1674,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -2782,9 +2833,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.88671875" customWidth="1"/>
     <col min="2" max="2" width="30.109375" customWidth="1"/>
@@ -2828,8 +2881,22 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
OpenWeather_GSheets_ReportBot: From REF with queues to REF with tabular data
</commit_message>
<xml_diff>
--- a/uipath-projects/OpenWeather_GSheets_ReportBot/Data/Config.xlsx
+++ b/uipath-projects/OpenWeather_GSheets_ReportBot/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Giancarlo\GitHub\automation-ai-portfolio\uipath-projects\OpenWeather_GSheets_ReportBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8FA837-9AA4-4188-8768-5D9FE803F132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A558FF63-FF8F-4384-B39A-CA9EEB25A899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -190,6 +190,24 @@
   </si>
   <si>
     <t>GSFolder</t>
+  </si>
+  <si>
+    <t>GoogleFileSheet</t>
+  </si>
+  <si>
+    <t>GoogleFileCell</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Sheet3</t>
+  </si>
+  <si>
+    <t>TestSpreadsheet</t>
+  </si>
+  <si>
+    <t>GoogleFile</t>
   </si>
 </sst>
 </file>
@@ -568,7 +586,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -669,9 +687,30 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
OpenWeather_GSheets_ReportBot: Integrated with Google Sheets and Weather API
</commit_message>
<xml_diff>
--- a/uipath-projects/OpenWeather_GSheets_ReportBot/Data/Config.xlsx
+++ b/uipath-projects/OpenWeather_GSheets_ReportBot/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Giancarlo\GitHub\automation-ai-portfolio\uipath-projects\OpenWeather_GSheets_ReportBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A558FF63-FF8F-4384-B39A-CA9EEB25A899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49322579-D784-42A0-AF9D-FB68C997871D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,56 +165,56 @@
     <t>WeatherAPIKey</t>
   </si>
   <si>
+    <t>GoogleCredential</t>
+  </si>
+  <si>
+    <t>InputCitiesPath</t>
+  </si>
+  <si>
+    <t>Data\InputCities.xlsx</t>
+  </si>
+  <si>
+    <t>InputCitiesFileSheet</t>
+  </si>
+  <si>
+    <t>Cities</t>
+  </si>
+  <si>
+    <t>OrchestratorFolderPath</t>
+  </si>
+  <si>
+    <t>GSFolder</t>
+  </si>
+  <si>
+    <t>GoogleFileSheet</t>
+  </si>
+  <si>
+    <t>GoogleFileCell</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>TestSpreadsheet</t>
+  </si>
+  <si>
+    <t>GoogleFile</t>
+  </si>
+  <si>
     <t>WeatherAPIKey_AssetName</t>
   </si>
   <si>
-    <t>GoogleCredential</t>
-  </si>
-  <si>
     <t>GoogleCredential_AssetName</t>
   </si>
   <si>
-    <t>InputCitiesPath</t>
-  </si>
-  <si>
-    <t>Data\InputCities.xlsx</t>
-  </si>
-  <si>
-    <t>InputCitiesFileSheet</t>
-  </si>
-  <si>
-    <t>Cities</t>
-  </si>
-  <si>
-    <t>OrchestratorFolderPath</t>
-  </si>
-  <si>
-    <t>GSFolder</t>
-  </si>
-  <si>
-    <t>GoogleFileSheet</t>
-  </si>
-  <si>
-    <t>GoogleFileCell</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>Sheet3</t>
-  </si>
-  <si>
-    <t>TestSpreadsheet</t>
-  </si>
-  <si>
-    <t>GoogleFile</t>
+    <t>Sheet4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -233,6 +233,13 @@
       <charset val="128"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -259,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -269,6 +276,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,7 +594,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -665,54 +673,68 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
         <v>59</v>
       </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2873,7 +2895,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2920,21 +2942,9 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2943,7 +2953,9 @@
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="C11" s="5"/>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3936,5 +3948,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OpenWeather_GSheets_ReportBot: Validation of Input Cities added
</commit_message>
<xml_diff>
--- a/uipath-projects/OpenWeather_GSheets_ReportBot/Data/Config.xlsx
+++ b/uipath-projects/OpenWeather_GSheets_ReportBot/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Giancarlo\GitHub\automation-ai-portfolio\uipath-projects\OpenWeather_GSheets_ReportBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49322579-D784-42A0-AF9D-FB68C997871D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4199E16D-F3B9-4329-930B-45BF03B99775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>Sheet4</t>
+  </si>
+  <si>
+    <t>ErrorFile</t>
+  </si>
+  <si>
+    <t>Data\ErrorFile.xlsx</t>
+  </si>
+  <si>
+    <t>ErrorFileSheet</t>
   </si>
 </sst>
 </file>
@@ -594,7 +603,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -735,8 +744,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>